<commit_message>
update the v2 template
</commit_message>
<xml_diff>
--- a/covid19_forecaster/data/templates/covid-budget-scenarios-v2.xlsx
+++ b/covid19_forecaster/data/templates/covid-budget-scenarios-v2.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/Projects/BudgetWork/Analysis/v2/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/Projects/BudgetWork/Analysis/v2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947EB449-E76F-A242-BD24-46D03678DDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CECA5E-DEEB-BC42-9741-AA463EBBE50F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36800" yWindow="1540" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35220" yWindow="820" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Normalized Declines" sheetId="2" r:id="rId2"/>
-    <sheet name="Budget Revenues" sheetId="4" r:id="rId3"/>
-    <sheet name="Optimistic (Raw)" sheetId="5" r:id="rId4"/>
-    <sheet name="Pessimistic (Raw)" sheetId="6" r:id="rId5"/>
-    <sheet name="Normalized Declines (Raw)" sheetId="7" r:id="rId6"/>
+    <sheet name="Budget Revenues" sheetId="3" r:id="rId3"/>
+    <sheet name="Normalized Declines (Raw)" sheetId="4" r:id="rId4"/>
+    <sheet name="Optimistic (Raw)" sheetId="5" r:id="rId5"/>
+    <sheet name="Pessimistic (Raw)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="66">
+  <si>
+    <t>Dollars in thousands</t>
+  </si>
   <si>
     <t>FY 2021</t>
   </si>
@@ -50,9 +53,6 @@
     <t>Tax</t>
   </si>
   <si>
-    <t>Baseline</t>
-  </si>
-  <si>
     <t>Optimistic</t>
   </si>
   <si>
@@ -62,31 +62,52 @@
     <t>Pessimisitic</t>
   </si>
   <si>
+    <t>Wage &amp; Earnings†</t>
+  </si>
+  <si>
+    <t>BIRT</t>
+  </si>
+  <si>
+    <t>Realty Transfer</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Parking</t>
+  </si>
+  <si>
+    <t>Net Profits†</t>
+  </si>
+  <si>
+    <t>Beverage</t>
+  </si>
+  <si>
     <t>Amusement</t>
   </si>
   <si>
-    <t>BIRT</t>
-  </si>
-  <si>
-    <t>Parking</t>
-  </si>
-  <si>
-    <t>Realty Transfer</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>† Includes both the City and PICA portions of the tax</t>
   </si>
   <si>
-    <t>Note: FY21 baseline from "Target Budget" totals in FY21 Q2 QCMR; FY22 baseline from Adopted FY21 - FY25 Five Year Financial Plan, June 2020</t>
-  </si>
-  <si>
-    <t>Forecasted Revenues Relative to Pre-COVID Baseline</t>
+    <t>Gross to City Sales Deductions</t>
+  </si>
+  <si>
+    <t>Deductions to convert from City+School District collections to just City collections</t>
+  </si>
+  <si>
+    <t>FY21</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>Note: from FYP 21-25 Sales Tax Model spreadsheet — see "fyp-numbers-backup.xlsx"</t>
+  </si>
+  <si>
+    <t>Quarterly Tax Revenue Totals as Percent of the Pre-COVID Baseline</t>
   </si>
   <si>
     <t>Actual</t>
@@ -122,9 +143,15 @@
     <t>FY22 Q4</t>
   </si>
   <si>
+    <t>Wage &amp; Earnings</t>
+  </si>
+  <si>
     <t>Net Profits</t>
   </si>
   <si>
+    <t>Note: The pre-COVID baseline is defined as the revenue level during the four quarters prior to the onset of the COVID pandemic in FY20 Q4</t>
+  </si>
+  <si>
     <t>tax</t>
   </si>
   <si>
@@ -179,9 +206,6 @@
     <t>NPT includes City &amp; PICA share of Net Profits Tax</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
     <t>kind</t>
   </si>
   <si>
@@ -194,75 +218,36 @@
     <t>severe</t>
   </si>
   <si>
-    <t>Beverage</t>
-  </si>
-  <si>
-    <r>
-      <t>Wage &amp; Earnings</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Open Sans Regular"/>
-      </rPr>
-      <t>†</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Net Profits</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Open Sans Regular"/>
-      </rPr>
-      <t>†</t>
-    </r>
-  </si>
-  <si>
-    <t>FY21</t>
-  </si>
-  <si>
-    <t>FY22</t>
-  </si>
-  <si>
-    <t>Gross to City Sales Deductions</t>
-  </si>
-  <si>
-    <t>Note: from FYP 21-25 Sales Tax Model spreadsheet — see "fyp-numbers-backup.xlsx"</t>
-  </si>
-  <si>
-    <t>Deductions to convert from City+School District collections to just City collections</t>
-  </si>
-  <si>
-    <t>Dollars in thousands</t>
-  </si>
-  <si>
-    <t>Estimated Tax Revenue Impacts for Major City of Philadelphia Taxes in Fiscal Years 2021 and 2022</t>
-  </si>
-  <si>
-    <t>Wage &amp; Earnings</t>
-  </si>
-  <si>
-    <t>Note: Pre-COVID baseline defined as revenue level during the four quarters prior to the onset of the COVID pandemic in FY20 Q4</t>
+    <t>all_taxes</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1: Revised Tax Revenue Impacts for Major City of Philadelphia Taxes </t>
+  </si>
+  <si>
+    <t>in Fiscal Years 2021 and 2022</t>
+  </si>
+  <si>
+    <t>Note: City Budget data reflects "Target Budget" totals in FY21 Q2 QCMR; FY22 baseline from Adopted FY21 - FY25 Five Year Financial Plan, June 2020</t>
+  </si>
+  <si>
+    <t>City Budget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,12 +290,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFCC3000"/>
-      <name val="Open Sans Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -334,32 +313,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3A833C"/>
-      <name val="Open Sans Regular"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Open Sans Regular"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Open Sans Regular"/>
     </font>
@@ -382,19 +336,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Open Sans Regular"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +344,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Open Sans Regular"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Open Sans Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFCC3000"/>
+      <name val="Open Sans Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
       <color theme="1"/>
       <name val="Open Sans Regular"/>
     </font>
@@ -421,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -505,15 +468,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -570,17 +524,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -904,19 +847,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -938,6 +868,87 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -948,105 +959,62 @@
   </cellStyleXfs>
   <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1055,173 +1023,216 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="5" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="6" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1233,7 +1244,7 @@
   <colors>
     <mruColors>
       <color rgb="FFCFCFCF"/>
-      <color rgb="FF3A833C"/>
+      <color rgb="FFCC3000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1571,494 +1582,544 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B3:J26"/>
+  <dimension ref="B3:J28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
-    <col min="3" max="10" width="13.83203125" style="1" customWidth="1"/>
-    <col min="11" max="24" width="8.83203125" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="4.33203125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="27" customWidth="1"/>
+    <col min="3" max="5" width="12.83203125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="27" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="27" customWidth="1"/>
+    <col min="8" max="8" width="14" style="27" customWidth="1"/>
+    <col min="9" max="10" width="12.83203125" style="27" customWidth="1"/>
+    <col min="11" max="25" width="8.83203125" style="27" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="20" thickBot="1"/>
+    <row r="3" spans="2:10" ht="20" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:10" ht="26" customHeight="1">
-      <c r="B4" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
-    </row>
-    <row r="5" spans="2:10" ht="25" customHeight="1">
-      <c r="B5" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="43"/>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="42"/>
-      <c r="C6" s="64" t="s">
+      <c r="B4" s="102" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
+    </row>
+    <row r="5" spans="2:10" ht="21" customHeight="1">
+      <c r="B5" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
+    </row>
+    <row r="6" spans="2:10" ht="25" customHeight="1">
+      <c r="B6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="65"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69" t="s">
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="2:10" ht="20" customHeight="1">
+      <c r="B7" s="29"/>
+      <c r="C7" s="109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="70"/>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="38" t="s">
+      <c r="G7" s="62"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="J7" s="110"/>
+    </row>
+    <row r="8" spans="2:10" ht="20" customHeight="1">
+      <c r="B8" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="C8" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="29" t="s">
+      <c r="F8" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H8" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I8" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J8" s="49" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="21">
-      <c r="B8" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="85">
+    <row r="9" spans="2:10" ht="22" customHeight="1">
+      <c r="B9" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="51">
         <f>'Budget Revenues'!C9</f>
         <v>2000565</v>
       </c>
-      <c r="D8" s="86">
+      <c r="D9" s="113">
         <f>'Optimistic (Raw)'!C9</f>
-        <v>1988130.246453841</v>
-      </c>
-      <c r="E8" s="87">
+        <v>1962993.1692271589</v>
+      </c>
+      <c r="E9" s="52">
         <f>'Pessimistic (Raw)'!C9</f>
-        <v>1934704.2015424131</v>
-      </c>
-      <c r="F8" s="88">
+        <v>1955840.2836242591</v>
+      </c>
+      <c r="F9" s="53">
         <f>'Budget Revenues'!E9</f>
         <v>2166518.7329019052</v>
       </c>
-      <c r="G8" s="86">
+      <c r="G9" s="113">
         <f>'Optimistic (Raw)'!D9</f>
-        <v>2092383.094440724</v>
-      </c>
-      <c r="H8" s="89">
+        <v>2094345.8161026461</v>
+      </c>
+      <c r="H9" s="114">
         <f>'Pessimistic (Raw)'!D9</f>
-        <v>1994961.6094716</v>
-      </c>
-      <c r="I8" s="90">
-        <f t="shared" ref="I8:I15" si="0">G8+D8-F8-C8</f>
-        <v>-86570.392007340211</v>
-      </c>
-      <c r="J8" s="91">
-        <f t="shared" ref="J8:J15" si="1">H8+E8-F8-C8</f>
-        <v>-237417.92188789183</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="92" t="s">
+        <v>2051070.841844277</v>
+      </c>
+      <c r="I9" s="115">
+        <f t="shared" ref="I9:I17" si="0">G9+D9-F9-C9</f>
+        <v>-109744.74757210026</v>
+      </c>
+      <c r="J9" s="54">
+        <f t="shared" ref="J9:J17" si="1">H9+E9-F9-C9</f>
+        <v>-160172.60743336892</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="22" customHeight="1">
+      <c r="B10" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="82">
+        <v>684288</v>
+      </c>
+      <c r="D10" s="83">
+        <f>C10</f>
+        <v>684288</v>
+      </c>
+      <c r="E10" s="84">
+        <f>C10</f>
+        <v>684288</v>
+      </c>
+      <c r="F10" s="85">
+        <v>731697</v>
+      </c>
+      <c r="G10" s="83">
+        <v>699204</v>
+      </c>
+      <c r="H10" s="86">
+        <f>G10</f>
+        <v>699204</v>
+      </c>
+      <c r="I10" s="116">
+        <f t="shared" si="0"/>
+        <v>-32493</v>
+      </c>
+      <c r="J10" s="87">
+        <f t="shared" si="1"/>
+        <v>-32493</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="20" customHeight="1">
+      <c r="B11" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C11" s="78">
         <f>'Budget Revenues'!C3</f>
         <v>482147</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D11" s="79">
         <f>'Optimistic (Raw)'!C3</f>
         <v>513128.15045075922</v>
       </c>
-      <c r="E9" s="95">
+      <c r="E11" s="56">
         <f>'Pessimistic (Raw)'!C3</f>
         <v>478518.61148725299</v>
       </c>
-      <c r="F9" s="96">
+      <c r="F11" s="80">
         <f>'Budget Revenues'!E3</f>
         <v>605916</v>
       </c>
-      <c r="G9" s="94">
+      <c r="G11" s="79">
         <f>'Optimistic (Raw)'!D3</f>
         <v>539850.19252898183</v>
       </c>
-      <c r="H9" s="97">
+      <c r="H11" s="57">
         <f>'Pessimistic (Raw)'!D3</f>
         <v>514143.04050379217</v>
       </c>
-      <c r="I9" s="98">
+      <c r="I11" s="115">
         <f t="shared" si="0"/>
         <v>-35084.65702025895</v>
       </c>
-      <c r="J9" s="99">
+      <c r="J11" s="54">
         <f t="shared" si="1"/>
         <v>-95401.348008954898</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="101">
+    <row r="12" spans="2:10" ht="20" customHeight="1">
+      <c r="B12" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="82">
         <f>'Budget Revenues'!C6</f>
         <v>292816</v>
       </c>
-      <c r="D10" s="102">
+      <c r="D12" s="83">
         <f>'Optimistic (Raw)'!C6</f>
         <v>332277.71716741187</v>
       </c>
-      <c r="E10" s="103">
+      <c r="E12" s="84">
         <f>'Pessimistic (Raw)'!C6</f>
         <v>309309.16141848691</v>
       </c>
-      <c r="F10" s="104">
+      <c r="F12" s="85">
         <f>'Budget Revenues'!E6</f>
         <v>301308</v>
       </c>
-      <c r="G10" s="102">
+      <c r="G12" s="83">
         <f>'Optimistic (Raw)'!D6</f>
         <v>358563.77458584151</v>
       </c>
-      <c r="H10" s="105">
+      <c r="H12" s="86">
         <f>'Pessimistic (Raw)'!D6</f>
         <v>313694.55911220011</v>
       </c>
-      <c r="I10" s="90">
+      <c r="I12" s="116">
         <f t="shared" si="0"/>
         <v>96717.491753253387</v>
       </c>
-      <c r="J10" s="91">
+      <c r="J12" s="87">
         <f t="shared" si="1"/>
         <v>28879.720530687016</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="92" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="93">
-        <f>'Budget Revenues'!C7 - C25</f>
+    <row r="13" spans="2:10" ht="20" customHeight="1">
+      <c r="B13" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="78">
+        <f>'Budget Revenues'!C7 - C27</f>
         <v>173876.16655304801</v>
       </c>
-      <c r="D11" s="94">
-        <f>'Optimistic (Raw)'!C7 - C25</f>
+      <c r="D13" s="79">
+        <f>'Optimistic (Raw)'!C7 - C27</f>
         <v>205342.3913346809</v>
       </c>
-      <c r="E11" s="95">
-        <f>'Pessimistic (Raw)'!C7 - C25</f>
+      <c r="E13" s="56">
+        <f>'Pessimistic (Raw)'!C7 - C27</f>
         <v>201019.97437850229</v>
       </c>
-      <c r="F11" s="96">
-        <f>'Budget Revenues'!E7 - C26</f>
+      <c r="F13" s="80">
+        <f>'Budget Revenues'!E7 - C28</f>
         <v>315121.01426197897</v>
       </c>
-      <c r="G11" s="94">
-        <f>'Optimistic (Raw)'!D7 - C26</f>
+      <c r="G13" s="79">
+        <f>'Optimistic (Raw)'!D7 - C28</f>
         <v>339683.71317785408</v>
       </c>
-      <c r="H11" s="97">
-        <f>'Pessimistic (Raw)'!D7 - C26</f>
+      <c r="H13" s="57">
+        <f>'Pessimistic (Raw)'!D7 - C28</f>
         <v>328491.53624475643</v>
       </c>
-      <c r="I11" s="98">
+      <c r="I13" s="115">
         <f t="shared" si="0"/>
         <v>56028.923697508057</v>
       </c>
-      <c r="J11" s="99">
+      <c r="J13" s="54">
         <f t="shared" si="1"/>
         <v>40514.329808231792</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="100" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="101">
+    <row r="14" spans="2:10" ht="20" customHeight="1">
+      <c r="B14" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="82">
         <f>'Budget Revenues'!C5</f>
         <v>61088</v>
       </c>
-      <c r="D12" s="102">
+      <c r="D14" s="83">
         <f>'Optimistic (Raw)'!C5</f>
         <v>52058.778690093699</v>
       </c>
-      <c r="E12" s="103">
+      <c r="E14" s="84">
         <f>'Pessimistic (Raw)'!C5</f>
         <v>49121.780516297891</v>
       </c>
-      <c r="F12" s="104">
+      <c r="F14" s="85">
         <f>'Budget Revenues'!E5</f>
         <v>83298</v>
       </c>
-      <c r="G12" s="102">
+      <c r="G14" s="83">
         <f>'Optimistic (Raw)'!D5</f>
         <v>83160.913900785905</v>
       </c>
-      <c r="H12" s="105">
+      <c r="H14" s="86">
         <f>'Pessimistic (Raw)'!D5</f>
         <v>70653.884547747002</v>
       </c>
-      <c r="I12" s="90">
+      <c r="I14" s="116">
         <f t="shared" si="0"/>
         <v>-9166.3074091204035</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J14" s="87">
         <f t="shared" si="1"/>
         <v>-24610.334935955107</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="21">
-      <c r="B13" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="96">
+    <row r="15" spans="2:10" ht="22" customHeight="1">
+      <c r="B15" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="80">
         <f>'Budget Revenues'!C4</f>
         <v>56218</v>
       </c>
-      <c r="D13" s="94">
+      <c r="D15" s="79">
         <f>'Optimistic (Raw)'!C4</f>
         <v>63119.264660570007</v>
       </c>
-      <c r="E13" s="95">
+      <c r="E15" s="56">
         <f>'Pessimistic (Raw)'!C4</f>
         <v>52771.23810704668</v>
       </c>
-      <c r="F13" s="96">
+      <c r="F15" s="80">
         <f>'Budget Revenues'!E4</f>
         <v>72252.784409516476</v>
       </c>
-      <c r="G13" s="94">
+      <c r="G15" s="79">
         <f>'Optimistic (Raw)'!D4</f>
         <v>69747.17724995059</v>
       </c>
-      <c r="H13" s="97">
+      <c r="H15" s="57">
         <f>'Pessimistic (Raw)'!D4</f>
         <v>65543.827594732618</v>
       </c>
-      <c r="I13" s="98">
+      <c r="I15" s="115">
         <f t="shared" si="0"/>
         <v>4395.657501004127</v>
       </c>
-      <c r="J13" s="99">
+      <c r="J15" s="54">
         <f t="shared" si="1"/>
         <v>-10155.718707737178</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="100" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="104">
+    <row r="16" spans="2:10" ht="20" customHeight="1">
+      <c r="B16" s="81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="85">
         <f>'Budget Revenues'!C8</f>
         <v>67441</v>
       </c>
-      <c r="D14" s="102">
+      <c r="D16" s="83">
         <f>'Optimistic (Raw)'!C8</f>
         <v>67932.599728931222</v>
       </c>
-      <c r="E14" s="103">
+      <c r="E16" s="84">
         <f>'Pessimistic (Raw)'!C8</f>
         <v>66080.899188435054</v>
       </c>
-      <c r="F14" s="104">
+      <c r="F16" s="85">
         <f>'Budget Revenues'!E8</f>
         <v>67954</v>
       </c>
-      <c r="G14" s="102">
+      <c r="G16" s="83">
         <f>'Optimistic (Raw)'!D8</f>
         <v>74103.478048825011</v>
       </c>
-      <c r="H14" s="105">
+      <c r="H16" s="86">
         <f>'Pessimistic (Raw)'!D8</f>
         <v>71863.599382376968</v>
       </c>
-      <c r="I14" s="90">
+      <c r="I16" s="116">
         <f t="shared" si="0"/>
         <v>6641.0777777562325</v>
       </c>
-      <c r="J14" s="91">
+      <c r="J16" s="87">
         <f t="shared" si="1"/>
         <v>2549.4985708120221</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B15" s="106" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="107">
+    <row r="17" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B17" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="95">
         <f>'Budget Revenues'!C2</f>
         <v>12818</v>
       </c>
-      <c r="D15" s="108">
+      <c r="D17" s="96">
         <f>'Optimistic (Raw)'!C2</f>
         <v>3073.877410478342</v>
       </c>
-      <c r="E15" s="109">
+      <c r="E17" s="97">
         <f>'Pessimistic (Raw)'!C2</f>
         <v>2372.2827102244878</v>
       </c>
-      <c r="F15" s="110">
+      <c r="F17" s="98">
         <f>'Budget Revenues'!E2</f>
         <v>26116</v>
       </c>
-      <c r="G15" s="108">
+      <c r="G17" s="96">
         <f>'Optimistic (Raw)'!D2</f>
         <v>19816.433954755132</v>
       </c>
-      <c r="H15" s="111">
+      <c r="H17" s="99">
         <f>'Pessimistic (Raw)'!D2</f>
         <v>15258.296771098911</v>
       </c>
-      <c r="I15" s="112">
+      <c r="I17" s="100">
         <f t="shared" si="0"/>
         <v>-16043.688634766528</v>
       </c>
-      <c r="J15" s="113">
+      <c r="J17" s="101">
         <f t="shared" si="1"/>
         <v>-21303.420518676601</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="20" customHeight="1" thickTop="1">
-      <c r="B16" s="114" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="115">
-        <f t="shared" ref="C16:J16" si="2">SUM(C8:C15)</f>
-        <v>3146969.166553048</v>
-      </c>
-      <c r="D16" s="116">
+    <row r="18" spans="2:10" ht="20" customHeight="1" thickTop="1">
+      <c r="B18" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="117">
+        <f t="shared" ref="C18:J18" si="2">SUM(C9:C17)</f>
+        <v>3831257.166553048</v>
+      </c>
+      <c r="D18" s="118">
         <f t="shared" si="2"/>
-        <v>3225063.0258967662</v>
-      </c>
-      <c r="E16" s="117">
+        <v>3884213.9486700837</v>
+      </c>
+      <c r="E18" s="89">
         <f t="shared" si="2"/>
-        <v>3093898.1493486594</v>
-      </c>
-      <c r="F16" s="118">
+        <v>3799322.2314305054</v>
+      </c>
+      <c r="F18" s="90">
         <f t="shared" si="2"/>
-        <v>3638484.5315734008</v>
-      </c>
-      <c r="G16" s="119">
+        <v>4370181.5315734008</v>
+      </c>
+      <c r="G18" s="91">
         <f t="shared" si="2"/>
-        <v>3577308.7778877188</v>
-      </c>
-      <c r="H16" s="120">
+        <v>4278475.4995496403</v>
+      </c>
+      <c r="H18" s="92">
         <f t="shared" si="2"/>
-        <v>3374610.3536283039</v>
-      </c>
-      <c r="I16" s="121">
+        <v>4129923.5860009808</v>
+      </c>
+      <c r="I18" s="119">
         <f t="shared" si="2"/>
-        <v>16918.105658035711</v>
-      </c>
-      <c r="J16" s="122">
+        <v>-38749.249906724333</v>
+      </c>
+      <c r="J18" s="93">
         <f t="shared" si="2"/>
-        <v>-316945.19514948473</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="20" customHeight="1">
-      <c r="B17" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="40"/>
-    </row>
-    <row r="18" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B18" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="41"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="32" t="s">
-        <v>59</v>
-      </c>
+        <v>-272192.88069496187</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="20" customHeight="1">
+      <c r="B19" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="122"/>
+    </row>
+    <row r="20" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B20" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="33">
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="58">
         <f>115890808/1000</f>
         <v>115890.808</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="34">
+    <row r="27" spans="2:10">
+      <c r="B27" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="59">
         <f>116522458/1000</f>
         <v>116522.458</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="31" t="s">
-        <v>58</v>
+    <row r="28" spans="2:10">
+      <c r="B28" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:J15">
-    <sortCondition descending="1" ref="F8:F15"/>
-  </sortState>
-  <mergeCells count="3">
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:J6"/>
+  <mergeCells count="5">
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2072,869 +2133,868 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="22" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="22" customWidth="1"/>
-    <col min="4" max="11" width="9.83203125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="19" customWidth="1"/>
+    <col min="4" max="11" width="9.83203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="16" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:12" ht="39" customHeight="1">
-      <c r="B2" s="74" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="76"/>
+      <c r="B2" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="72"/>
     </row>
     <row r="3" spans="2:12" ht="20" customHeight="1">
-      <c r="B3" s="19"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="15"/>
+      <c r="D3" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="62"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="63"/>
     </row>
     <row r="4" spans="2:12" ht="22" customHeight="1">
-      <c r="B4" s="20"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="55" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="62" t="s">
+      <c r="E4" s="36" t="s">
         <v>27</v>
       </c>
+      <c r="F4" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="43" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="2:12" ht="19" customHeight="1">
-      <c r="B5" s="79" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="57" t="s">
+      <c r="B5" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="41">
         <f>'Normalized Declines (Raw)'!D23</f>
         <v>0.9213965682080032</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="41">
         <f>'Normalized Declines (Raw)'!E23</f>
         <v>0.9356056139462301</v>
       </c>
-      <c r="F5" s="61">
+      <c r="F5" s="42">
         <f>'Normalized Declines (Raw)'!F23</f>
         <v>0.87980321339352341</v>
       </c>
-      <c r="G5" s="60">
+      <c r="G5" s="41">
         <f>'Normalized Declines (Raw)'!G24</f>
-        <v>0.89356372527232952</v>
-      </c>
-      <c r="H5" s="60">
+        <v>0.87339073337913475</v>
+      </c>
+      <c r="H5" s="41">
         <f>'Normalized Declines (Raw)'!H24</f>
-        <v>0.94572412477475598</v>
-      </c>
-      <c r="I5" s="60">
+        <v>0.92074759596716416</v>
+      </c>
+      <c r="I5" s="41">
         <f>'Normalized Declines (Raw)'!I24</f>
-        <v>0.96700588431045986</v>
-      </c>
-      <c r="J5" s="60">
+        <v>0.95058492075138856</v>
+      </c>
+      <c r="J5" s="41">
         <f>'Normalized Declines (Raw)'!J24</f>
-        <v>0.95620143147246406</v>
-      </c>
-      <c r="K5" s="60">
+        <v>0.95791588696615193</v>
+      </c>
+      <c r="K5" s="41">
         <f>'Normalized Declines (Raw)'!K24</f>
-        <v>0.94117637444183477</v>
-      </c>
-      <c r="L5" s="63">
+        <v>0.95501099482379692</v>
+      </c>
+      <c r="L5" s="44">
         <f>'Normalized Declines (Raw)'!L24</f>
-        <v>1.004745470365263</v>
+        <v>1.0074311136596641</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="19" customHeight="1">
-      <c r="B6" s="80"/>
-      <c r="C6" s="58" t="s">
+      <c r="B6" s="75"/>
+      <c r="C6" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="21">
         <f>'Normalized Declines (Raw)'!D23</f>
         <v>0.9213965682080032</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="21">
         <f>'Normalized Declines (Raw)'!E23</f>
         <v>0.9356056139462301</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="7">
         <f>'Normalized Declines (Raw)'!F23</f>
         <v>0.87980321339352341</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="21">
         <f>'Normalized Declines (Raw)'!G25</f>
-        <v>0.84493275045896465</v>
-      </c>
-      <c r="H6" s="27">
+        <v>0.86910210149954803</v>
+      </c>
+      <c r="H6" s="21">
         <f>'Normalized Declines (Raw)'!H25</f>
-        <v>0.89923971011504922</v>
-      </c>
-      <c r="I6" s="27">
+        <v>0.91197560070142802</v>
+      </c>
+      <c r="I6" s="21">
         <f>'Normalized Declines (Raw)'!I25</f>
-        <v>0.91238917500026184</v>
-      </c>
-      <c r="J6" s="27">
+        <v>0.93739798411844588</v>
+      </c>
+      <c r="J6" s="21">
         <f>'Normalized Declines (Raw)'!J25</f>
-        <v>0.91549146302094686</v>
-      </c>
-      <c r="K6" s="27">
+        <v>0.9395616359029878</v>
+      </c>
+      <c r="K6" s="21">
         <f>'Normalized Declines (Raw)'!K25</f>
-        <v>0.90476275832553921</v>
-      </c>
-      <c r="L6" s="16">
+        <v>0.93353918965308891</v>
+      </c>
+      <c r="L6" s="12">
         <f>'Normalized Declines (Raw)'!L25</f>
-        <v>0.95524557678015487</v>
+        <v>0.98065537933534308</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="19" customHeight="1">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <f>'Normalized Declines (Raw)'!D5</f>
         <v>1.031145156376116</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="8">
         <f>'Normalized Declines (Raw)'!E5</f>
         <v>1.4414276454789421</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="18">
         <f>'Normalized Declines (Raw)'!F5</f>
         <v>1.2942611111301059</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="8">
         <f>'Normalized Declines (Raw)'!G6</f>
         <v>0.93</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="8">
         <f>'Normalized Declines (Raw)'!H6</f>
         <v>0.92999999999999994</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="8">
         <f>'Normalized Declines (Raw)'!I6</f>
         <v>1.05</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="8">
         <f>'Normalized Declines (Raw)'!J6</f>
         <v>1.05</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="8">
         <f>'Normalized Declines (Raw)'!K6</f>
         <v>1.05</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="13">
         <f>'Normalized Declines (Raw)'!L6</f>
         <v>1.05</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="19" customHeight="1">
-      <c r="B8" s="80"/>
-      <c r="C8" s="58" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="9">
         <f>D7</f>
         <v>1.031145156376116</v>
       </c>
-      <c r="E8" s="13">
-        <f t="shared" ref="E8:F8" si="0">E7</f>
+      <c r="E8" s="9">
+        <f>E7</f>
         <v>1.4414276454789421</v>
       </c>
-      <c r="F8" s="14">
-        <f t="shared" si="0"/>
+      <c r="F8" s="10">
+        <f>F7</f>
         <v>1.2942611111301059</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="9">
         <f>'Normalized Declines (Raw)'!G7</f>
         <v>0.84999999999999987</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="9">
         <f>'Normalized Declines (Raw)'!H7</f>
         <v>0.85</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="9">
         <f>'Normalized Declines (Raw)'!I7</f>
         <v>1</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="9">
         <f>'Normalized Declines (Raw)'!J7</f>
         <v>1</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="9">
         <f>'Normalized Declines (Raw)'!K7</f>
         <v>1</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <f>'Normalized Declines (Raw)'!L7</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="19" customHeight="1">
-      <c r="B9" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="57" t="s">
+      <c r="B9" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="8">
         <f>'Normalized Declines (Raw)'!D14</f>
         <v>0.42683409348331569</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="8">
         <f>'Normalized Declines (Raw)'!E14</f>
         <v>0.90926752456581872</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="18">
         <f>'Normalized Declines (Raw)'!F14</f>
         <v>0.92869196085369443</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="8">
         <f>'Normalized Declines (Raw)'!G15</f>
         <v>0.82706183516301757</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="8">
         <f>'Normalized Declines (Raw)'!H15</f>
         <v>0.85700943397514917</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="8">
         <f>'Normalized Declines (Raw)'!I15</f>
         <v>0.98500839616036118</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="8">
         <f>'Normalized Declines (Raw)'!J15</f>
         <v>0.90376561439449232</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="8">
         <f>'Normalized Declines (Raw)'!K15</f>
         <v>0.94002631370113798</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="13">
         <f>'Normalized Declines (Raw)'!L15</f>
         <v>0.97046544138731294</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="19" customHeight="1">
-      <c r="B10" s="80"/>
-      <c r="C10" s="58" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="9">
         <f>D9</f>
         <v>0.42683409348331569</v>
       </c>
-      <c r="E10" s="13">
-        <f t="shared" ref="E10:F10" si="1">E9</f>
+      <c r="E10" s="9">
+        <f>E9</f>
         <v>0.90926752456581872</v>
       </c>
-      <c r="F10" s="14">
-        <f t="shared" si="1"/>
+      <c r="F10" s="10">
+        <f>F9</f>
         <v>0.92869196085369443</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="9">
         <f>'Normalized Declines (Raw)'!G16</f>
         <v>0.71313138806741372</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="9">
         <f>'Normalized Declines (Raw)'!H16</f>
         <v>0.7312871591927006</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="9">
         <f>'Normalized Declines (Raw)'!I16</f>
         <v>0.87379977941807407</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="9">
         <f>'Normalized Declines (Raw)'!J16</f>
         <v>0.79364170509002629</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="9">
         <f>'Normalized Declines (Raw)'!K16</f>
         <v>0.81916678753298589</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <f>'Normalized Declines (Raw)'!L16</f>
         <v>0.83804628101221312</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="19" customHeight="1">
-      <c r="B11" s="79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="57" t="s">
+      <c r="B11" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="8">
         <f>'Normalized Declines (Raw)'!D17</f>
         <v>0.73207738350268114</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="8">
         <f>'Normalized Declines (Raw)'!E17</f>
         <v>0.89691193138054093</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="18">
         <f>'Normalized Declines (Raw)'!F17</f>
         <v>0.94268362605282119</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="8">
         <f>'Normalized Declines (Raw)'!G18</f>
         <v>0.90760054031924198</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="8">
         <f>'Normalized Declines (Raw)'!H18</f>
         <v>0.92893204425860254</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="8">
         <f>'Normalized Declines (Raw)'!I18</f>
         <v>0.95021751350044359</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="8">
         <f>'Normalized Declines (Raw)'!J18</f>
         <v>0.96457659424785724</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="8">
         <f>'Normalized Declines (Raw)'!K18</f>
         <v>0.97865464369440747</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="13">
         <f>'Normalized Declines (Raw)'!L18</f>
         <v>0.98581445673850054</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="19" customHeight="1">
-      <c r="B12" s="80"/>
-      <c r="C12" s="58" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="9">
         <f>D11</f>
         <v>0.73207738350268114</v>
       </c>
-      <c r="E12" s="13">
-        <f t="shared" ref="E12:F12" si="2">E11</f>
+      <c r="E12" s="9">
+        <f>E11</f>
         <v>0.89691193138054093</v>
       </c>
-      <c r="F12" s="14">
-        <f t="shared" si="2"/>
+      <c r="F12" s="10">
+        <f>F11</f>
         <v>0.94268362605282119</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="9">
         <f>'Normalized Declines (Raw)'!G19</f>
         <v>0.89341884493725143</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="9">
         <f>'Normalized Declines (Raw)'!H19</f>
         <v>0.89339806638790387</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="9">
         <f>'Normalized Declines (Raw)'!I19</f>
         <v>0.91464305789358569</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="9">
         <f>'Normalized Declines (Raw)'!J19</f>
         <v>0.92915318849571427</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="9">
         <f>'Normalized Declines (Raw)'!K19</f>
         <v>0.95029125293042649</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="14">
         <f>'Normalized Declines (Raw)'!L19</f>
         <v>0.95737325049855149</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="19" customHeight="1">
-      <c r="B13" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="57" t="s">
+      <c r="B13" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="8">
         <f>'Normalized Declines (Raw)'!D11</f>
         <v>0.28912873120996158</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="8">
         <f>'Normalized Declines (Raw)'!E11</f>
         <v>0.3195025610644488</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="18">
         <f>'Normalized Declines (Raw)'!F11</f>
         <v>0.433306055149001</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="8">
         <f>'Normalized Declines (Raw)'!G12</f>
         <v>0.5</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="8">
         <f>'Normalized Declines (Raw)'!H12</f>
         <v>0.6</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="8">
         <f>'Normalized Declines (Raw)'!I12</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="8">
         <f>'Normalized Declines (Raw)'!J12</f>
         <v>0.8</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="8">
         <f>'Normalized Declines (Raw)'!K12</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="13">
         <f>'Normalized Declines (Raw)'!L12</f>
         <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="19" customHeight="1">
-      <c r="B14" s="80"/>
-      <c r="C14" s="58" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="9">
         <f>D13</f>
         <v>0.28912873120996158</v>
       </c>
-      <c r="E14" s="13">
-        <f t="shared" ref="E14:F14" si="3">E13</f>
+      <c r="E14" s="9">
+        <f>E13</f>
         <v>0.3195025610644488</v>
       </c>
-      <c r="F14" s="14">
-        <f t="shared" si="3"/>
+      <c r="F14" s="10">
+        <f>F13</f>
         <v>0.433306055149001</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="9">
         <f>'Normalized Declines (Raw)'!G13</f>
         <v>0.5</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="9">
         <f>'Normalized Declines (Raw)'!H13</f>
         <v>0.5</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="9">
         <f>'Normalized Declines (Raw)'!I13</f>
         <v>0.6</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="9">
         <f>'Normalized Declines (Raw)'!J13</f>
         <v>0.7</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="9">
         <f>'Normalized Declines (Raw)'!K13</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="14">
         <f>'Normalized Declines (Raw)'!L13</f>
         <v>0.80000000000000016</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="19" customHeight="1">
-      <c r="B15" s="79" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="57" t="s">
+      <c r="B15" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="8">
         <f>'Normalized Declines (Raw)'!D8</f>
         <v>0.64229998131242638</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="8">
         <f>'Normalized Declines (Raw)'!E8</f>
         <v>3.2970748140514292</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="18">
         <f>'Normalized Declines (Raw)'!F8</f>
         <v>0.91115097661055744</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="8">
         <f>'Normalized Declines (Raw)'!G9</f>
         <v>0.6</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="8">
         <f>'Normalized Declines (Raw)'!H9</f>
         <v>0.6</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="8">
         <f>'Normalized Declines (Raw)'!I9</f>
         <v>1</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="8">
         <f>'Normalized Declines (Raw)'!J9</f>
         <v>1.02</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="8">
         <f>'Normalized Declines (Raw)'!K9</f>
         <v>1.02</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="13">
         <f>'Normalized Declines (Raw)'!L9</f>
         <v>1.05</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="19" customHeight="1">
-      <c r="B16" s="80"/>
-      <c r="C16" s="58" t="s">
+      <c r="B16" s="75"/>
+      <c r="C16" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="9">
         <f>D15</f>
         <v>0.64229998131242638</v>
       </c>
-      <c r="E16" s="13">
-        <f t="shared" ref="E16:F16" si="4">E15</f>
+      <c r="E16" s="9">
+        <f>E15</f>
         <v>3.2970748140514292</v>
       </c>
-      <c r="F16" s="14">
-        <f t="shared" si="4"/>
+      <c r="F16" s="10">
+        <f>F15</f>
         <v>0.91115097661055744</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="9">
         <f>'Normalized Declines (Raw)'!G10</f>
         <v>0.4</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="9">
         <f>'Normalized Declines (Raw)'!H10</f>
         <v>0.4</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="9">
         <f>'Normalized Declines (Raw)'!I10</f>
         <v>0.98</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="9">
         <f>'Normalized Declines (Raw)'!J10</f>
         <v>0.98</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="9">
         <f>'Normalized Declines (Raw)'!K10</f>
         <v>0.98</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="14">
         <f>'Normalized Declines (Raw)'!L10</f>
         <v>0.97</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="19" customHeight="1">
-      <c r="B17" s="79" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="57" t="s">
+      <c r="B17" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="8">
         <f>'Normalized Declines (Raw)'!D20</f>
         <v>0.69603976309517057</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="8">
         <f>'Normalized Declines (Raw)'!E20</f>
         <v>0.86666239616362983</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="18">
         <f>'Normalized Declines (Raw)'!F20</f>
         <v>0.87338516924459131</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="8">
         <f>'Normalized Declines (Raw)'!G21</f>
         <v>0.9</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="8">
         <f>'Normalized Declines (Raw)'!H21</f>
         <v>0.9</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="8">
         <f>'Normalized Declines (Raw)'!I21</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="8">
         <f>'Normalized Declines (Raw)'!J21</f>
         <v>0.95</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="8">
         <f>'Normalized Declines (Raw)'!K21</f>
         <v>0.97</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L17" s="13">
         <f>'Normalized Declines (Raw)'!L21</f>
         <v>0.99</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="19" customHeight="1">
-      <c r="B18" s="80"/>
-      <c r="C18" s="58" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="9">
         <f>D17</f>
         <v>0.69603976309517057</v>
       </c>
-      <c r="E18" s="13">
-        <f t="shared" ref="E18:F18" si="5">E17</f>
+      <c r="E18" s="9">
+        <f>E17</f>
         <v>0.86666239616362983</v>
       </c>
-      <c r="F18" s="14">
-        <f t="shared" si="5"/>
+      <c r="F18" s="10">
+        <f>F17</f>
         <v>0.87338516924459131</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="9">
         <f>'Normalized Declines (Raw)'!G22</f>
         <v>0.85</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="9">
         <f>'Normalized Declines (Raw)'!H22</f>
         <v>0.85</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="9">
         <f>'Normalized Declines (Raw)'!I22</f>
         <v>0.9</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="9">
         <f>'Normalized Declines (Raw)'!J22</f>
         <v>0.92500000000000004</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="9">
         <f>'Normalized Declines (Raw)'!K22</f>
         <v>0.95</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="14">
         <f>'Normalized Declines (Raw)'!L22</f>
         <v>0.96999999999999986</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="19" customHeight="1">
-      <c r="B19" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="57" t="s">
+      <c r="B19" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="8">
         <f>'Normalized Declines (Raw)'!D2</f>
         <v>6.3142865794127284E-2</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="8">
         <f>'Normalized Declines (Raw)'!E2</f>
         <v>5.0199695405670902E-3</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="18">
         <f>'Normalized Declines (Raw)'!F2</f>
         <v>7.7731866953624371E-2</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="8">
         <f>'Normalized Declines (Raw)'!G3</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="8">
         <f>'Normalized Declines (Raw)'!H3</f>
         <v>0.3</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="8">
         <f>'Normalized Declines (Raw)'!I3</f>
         <v>0.5</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="8">
         <f>'Normalized Declines (Raw)'!J3</f>
         <v>0.7</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="8">
         <f>'Normalized Declines (Raw)'!K3</f>
         <v>0.9</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19" s="13">
         <f>'Normalized Declines (Raw)'!L3</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="19" customHeight="1">
-      <c r="B20" s="80"/>
-      <c r="C20" s="58" t="s">
+      <c r="B20" s="75"/>
+      <c r="C20" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="9">
         <f>D19</f>
         <v>6.3142865794127284E-2</v>
       </c>
-      <c r="E20" s="13">
-        <f t="shared" ref="E20:F20" si="6">E19</f>
+      <c r="E20" s="9">
+        <f>E19</f>
         <v>5.0199695405670902E-3</v>
       </c>
-      <c r="F20" s="14">
-        <f t="shared" si="6"/>
+      <c r="F20" s="10">
+        <f>F19</f>
         <v>7.7731866953624371E-2</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="9">
         <f>'Normalized Declines (Raw)'!G4</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="9">
         <f>'Normalized Declines (Raw)'!H4</f>
         <v>0.2</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="9">
         <f>'Normalized Declines (Raw)'!I4</f>
         <v>0.3</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="9">
         <f>'Normalized Declines (Raw)'!J4</f>
         <v>0.5</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="9">
         <f>'Normalized Declines (Raw)'!K4</f>
         <v>0.7</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="14">
         <f>'Normalized Declines (Raw)'!L4</f>
         <v>0.9</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="19" customHeight="1">
-      <c r="B21" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="59" t="s">
+      <c r="B21" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="22">
         <f>'Normalized Declines (Raw)'!D26</f>
-        <v>0.86424547635730642</v>
-      </c>
-      <c r="E21" s="28">
+        <v>0.8642454763573062</v>
+      </c>
+      <c r="E21" s="22">
         <f>'Normalized Declines (Raw)'!E26</f>
-        <v>0.93931372717126993</v>
-      </c>
-      <c r="F21" s="15">
+        <v>0.93931372717126982</v>
+      </c>
+      <c r="F21" s="11">
         <f>'Normalized Declines (Raw)'!F26</f>
         <v>0.89538487727018501</v>
       </c>
-      <c r="G21" s="28">
+      <c r="G21" s="22">
         <f>'Normalized Declines (Raw)'!G27</f>
-        <v>0.87215669335447066</v>
-      </c>
-      <c r="H21" s="28">
+        <v>0.85903936299714301</v>
+      </c>
+      <c r="H21" s="22">
         <f>'Normalized Declines (Raw)'!H27</f>
-        <v>0.90613687436761492</v>
-      </c>
-      <c r="I21" s="28">
+        <v>0.89485678551708547</v>
+      </c>
+      <c r="I21" s="22">
         <f>'Normalized Declines (Raw)'!I27</f>
-        <v>0.95735635458034407</v>
-      </c>
-      <c r="J21" s="28">
+        <v>0.94662610516975831</v>
+      </c>
+      <c r="J21" s="22">
         <f>'Normalized Declines (Raw)'!J27</f>
-        <v>0.95045833770876909</v>
-      </c>
-      <c r="K21" s="28">
+        <v>0.95157129206988267</v>
+      </c>
+      <c r="K21" s="22">
         <f>'Normalized Declines (Raw)'!K27</f>
-        <v>0.95447768841398661</v>
-      </c>
-      <c r="L21" s="21">
+        <v>0.96348256887667472</v>
+      </c>
+      <c r="L21" s="17">
         <f>'Normalized Declines (Raw)'!L27</f>
-        <v>1.013103464315301</v>
+        <v>1.0143159164944151</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="19" customHeight="1">
-      <c r="B22" s="82"/>
-      <c r="C22" s="58" t="s">
+      <c r="B22" s="75"/>
+      <c r="C22" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="9">
         <f>D21</f>
-        <v>0.86424547635730642</v>
-      </c>
-      <c r="E22" s="13">
+        <v>0.8642454763573062</v>
+      </c>
+      <c r="E22" s="9">
         <f>E21</f>
-        <v>0.93931372717126993</v>
-      </c>
-      <c r="F22" s="14">
+        <v>0.93931372717126982</v>
+      </c>
+      <c r="F22" s="10">
         <f>F21</f>
         <v>0.89538487727018501</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="9">
         <f>'Normalized Declines (Raw)'!G28</f>
-        <v>0.817604109991656</v>
-      </c>
-      <c r="H22" s="13">
+        <v>0.83332004165911022</v>
+      </c>
+      <c r="H22" s="9">
         <f>'Normalized Declines (Raw)'!H28</f>
-        <v>0.83621131789626324</v>
-      </c>
-      <c r="I22" s="13">
+        <v>0.84196319713103152</v>
+      </c>
+      <c r="I22" s="9">
         <f>'Normalized Declines (Raw)'!I28</f>
-        <v>0.8959308898051539</v>
-      </c>
-      <c r="J22" s="13">
+        <v>0.91227285161114025</v>
+      </c>
+      <c r="J22" s="9">
         <f>'Normalized Declines (Raw)'!J28</f>
-        <v>0.89935761689068849</v>
-      </c>
-      <c r="K22" s="13">
+        <v>0.91498298831646119</v>
+      </c>
+      <c r="K22" s="9">
         <f>'Normalized Declines (Raw)'!K28</f>
-        <v>0.90409275487043739</v>
-      </c>
-      <c r="L22" s="18">
+        <v>0.92282318021591314</v>
+      </c>
+      <c r="L22" s="14">
         <f>'Normalized Declines (Raw)'!L28</f>
-        <v>0.95579981083366627</v>
+        <v>0.96727124136322284</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="28" customHeight="1" thickBot="1">
-      <c r="B23" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="73"/>
+      <c r="B23" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2963,14 +3023,11 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D7:E7 F7 D9:F9 D11:F11 D13:F13 D15:F15 D17:F17 D19:F19 D21:F21" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2982,223 +3039,223 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="8" customWidth="1"/>
-    <col min="2" max="3" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="19" width="10.83203125" style="8" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="10.83203125" style="5" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="20" width="10.83203125" style="5" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2">
         <v>2020</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="5">
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2">
         <v>2022</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3">
         <v>18446</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="3">
         <v>12818</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>16611</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
         <v>26116</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3">
         <v>534239</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>482147</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>464321</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>605916</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3">
         <v>47354</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>56218</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>56218</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>72252.784409516476</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3">
         <v>77266</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>61088</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>76719</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>83298</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3">
         <v>319794</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>292816</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>292816</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <f>284410+16898</f>
         <v>301308</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3">
         <f>329466327/1000</f>
         <v>329466.32699999999</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <f>290398624.553048/1000</f>
         <v>290398.62455304799</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <f>290398624.553048/1000</f>
         <v>290398.62455304799</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <f>315121014.261979/1000</f>
         <v>315121.01426197897</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3">
         <v>69921</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>67441</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>67441</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <v>67954</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3">
         <v>2115404</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>2000565</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>2000565</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="3">
         <v>2166518.7329019052</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="6">
+      <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3">
         <v>204591</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>174508</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>174508</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="3">
         <f>159299+39299</f>
         <v>198598</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7" t="s">
-        <v>40</v>
+      <c r="A14" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="8" t="s">
-        <v>41</v>
+      <c r="A15" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="9" t="s">
-        <v>42</v>
+      <c r="A16" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="8" t="s">
-        <v>43</v>
+      <c r="A17" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="7" t="s">
-        <v>44</v>
+      <c r="A19" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="8" t="s">
-        <v>45</v>
+      <c r="A20" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="8" t="s">
-        <v>46</v>
+      <c r="A21" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3207,365 +3264,57 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="24">
-        <v>2020</v>
-      </c>
-      <c r="C1" s="24">
-        <v>2021</v>
-      </c>
-      <c r="D1" s="24">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>19922.471000000001</v>
-      </c>
-      <c r="C2">
-        <v>3073.877410478342</v>
-      </c>
-      <c r="D2">
-        <v>19816.433954755132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>526058.97600000002</v>
-      </c>
-      <c r="C3">
-        <v>513128.15045075922</v>
-      </c>
-      <c r="D3">
-        <v>539850.19252898183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4">
-        <v>47354.067999999999</v>
-      </c>
-      <c r="C4">
-        <v>63119.264660570007</v>
-      </c>
-      <c r="D4">
-        <v>69747.17724995059</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
-        <v>81377.207999999999</v>
-      </c>
-      <c r="C5">
-        <v>52058.778690093699</v>
-      </c>
-      <c r="D5">
-        <v>83160.913900785905</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6">
-        <v>311336.77399999998</v>
-      </c>
-      <c r="C6">
-        <v>332277.71716741187</v>
-      </c>
-      <c r="D6">
-        <v>358563.77458584151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7">
-        <v>329466.32699999999</v>
-      </c>
-      <c r="C7">
-        <v>321864.84933468088</v>
-      </c>
-      <c r="D7">
-        <v>339683.71317785408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="24" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
-        <v>71176.005999999994</v>
-      </c>
-      <c r="C8">
-        <v>67932.599728931222</v>
-      </c>
-      <c r="D8">
-        <v>74103.478048825011</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9">
-        <v>2132447.2349999999</v>
-      </c>
-      <c r="C9">
-        <v>1988130.246453841</v>
-      </c>
-      <c r="D9">
-        <v>2092383.094440724</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10">
-        <v>3519139.0649999999</v>
-      </c>
-      <c r="C10">
-        <v>3341585.4838967659</v>
-      </c>
-      <c r="D10">
-        <v>3577308.7778877169</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="24">
-        <v>2020</v>
-      </c>
-      <c r="C1" s="24">
-        <v>2021</v>
-      </c>
-      <c r="D1" s="24">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>19922.471000000001</v>
-      </c>
-      <c r="C2">
-        <v>2372.2827102244878</v>
-      </c>
-      <c r="D2">
-        <v>15258.296771098911</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>526058.97600000002</v>
-      </c>
-      <c r="C3">
-        <v>478518.61148725299</v>
-      </c>
-      <c r="D3">
-        <v>514143.04050379217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4">
-        <v>47354.067999999999</v>
-      </c>
-      <c r="C4">
-        <v>52771.23810704668</v>
-      </c>
-      <c r="D4">
-        <v>65543.827594732618</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
-        <v>81377.207999999999</v>
-      </c>
-      <c r="C5">
-        <v>49121.780516297891</v>
-      </c>
-      <c r="D5">
-        <v>70653.884547747002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6">
-        <v>311336.77399999998</v>
-      </c>
-      <c r="C6">
-        <v>309309.16141848691</v>
-      </c>
-      <c r="D6">
-        <v>313694.55911220011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7">
-        <v>329466.32699999999</v>
-      </c>
-      <c r="C7">
-        <v>317542.43237850227</v>
-      </c>
-      <c r="D7">
-        <v>328491.53624475643</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8">
-        <v>71176.005999999994</v>
-      </c>
-      <c r="C8">
-        <v>66080.899188435054</v>
-      </c>
-      <c r="D8">
-        <v>71863.599382376968</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9">
-        <v>2132447.2349999999</v>
-      </c>
-      <c r="C9">
-        <v>1934704.2015424131</v>
-      </c>
-      <c r="D9">
-        <v>1994961.6094716</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10">
-        <v>3519139.0649999999</v>
-      </c>
-      <c r="C10">
-        <v>3210420.60734866</v>
-      </c>
-      <c r="D10">
-        <v>3374610.3536283029</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:L1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="53">
+      <c r="B1" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="61">
         <v>43831</v>
       </c>
-      <c r="D1" s="53">
+      <c r="D1" s="61">
         <v>43922</v>
       </c>
-      <c r="E1" s="53">
+      <c r="E1" s="61">
         <v>44013</v>
       </c>
-      <c r="F1" s="53">
+      <c r="F1" s="61">
         <v>44105</v>
       </c>
-      <c r="G1" s="53">
+      <c r="G1" s="61">
         <v>44197</v>
       </c>
-      <c r="H1" s="53">
+      <c r="H1" s="61">
         <v>44287</v>
       </c>
-      <c r="I1" s="53">
+      <c r="I1" s="61">
         <v>44378</v>
       </c>
-      <c r="J1" s="53">
+      <c r="J1" s="61">
         <v>44470</v>
       </c>
-      <c r="K1" s="53">
+      <c r="K1" s="61">
         <v>44562</v>
       </c>
-      <c r="L1" s="53">
+      <c r="L1" s="61">
         <v>44652</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>49</v>
+      <c r="A2" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C2">
         <v>1.0442411563272469</v>
@@ -3581,9 +3330,9 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="83"/>
-      <c r="B3" s="24" t="s">
-        <v>50</v>
+      <c r="A3" s="77"/>
+      <c r="B3" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3617,9 +3366,9 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="83"/>
-      <c r="B4" s="24" t="s">
-        <v>51</v>
+      <c r="A4" s="77"/>
+      <c r="B4" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3653,11 +3402,11 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>49</v>
+      <c r="A5" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C5">
         <v>0.84796488485308497</v>
@@ -3673,9 +3422,9 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="83"/>
-      <c r="B6" s="24" t="s">
-        <v>50</v>
+      <c r="A6" s="77"/>
+      <c r="B6" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3709,9 +3458,9 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="83"/>
-      <c r="B7" s="24" t="s">
-        <v>51</v>
+      <c r="A7" s="77"/>
+      <c r="B7" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3745,11 +3494,11 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>49</v>
+      <c r="A8" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C8">
         <v>0.85596792203675143</v>
@@ -3765,9 +3514,9 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="83"/>
-      <c r="B9" s="24" t="s">
-        <v>50</v>
+      <c r="A9" s="77"/>
+      <c r="B9" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3801,9 +3550,9 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="83"/>
-      <c r="B10" s="24" t="s">
-        <v>51</v>
+      <c r="A10" s="77"/>
+      <c r="B10" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3837,11 +3586,11 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>49</v>
+      <c r="A11" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C11">
         <v>0.99268578081270098</v>
@@ -3857,9 +3606,9 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="83"/>
-      <c r="B12" s="24" t="s">
-        <v>50</v>
+      <c r="A12" s="77"/>
+      <c r="B12" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3893,9 +3642,9 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="83"/>
-      <c r="B13" s="24" t="s">
-        <v>51</v>
+      <c r="A13" s="77"/>
+      <c r="B13" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3929,11 +3678,11 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>49</v>
+      <c r="A14" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C14">
         <v>0.98062664266169686</v>
@@ -3949,9 +3698,9 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="83"/>
-      <c r="B15" s="24" t="s">
-        <v>50</v>
+      <c r="A15" s="77"/>
+      <c r="B15" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3985,9 +3734,9 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="83"/>
-      <c r="B16" s="24" t="s">
-        <v>51</v>
+      <c r="A16" s="77"/>
+      <c r="B16" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -4021,11 +3770,11 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>49</v>
+      <c r="A17" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C17">
         <v>0.97889123538588951</v>
@@ -4041,9 +3790,9 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="83"/>
-      <c r="B18" s="24" t="s">
-        <v>50</v>
+      <c r="A18" s="77"/>
+      <c r="B18" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -4077,9 +3826,9 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="83"/>
-      <c r="B19" s="24" t="s">
-        <v>51</v>
+      <c r="A19" s="77"/>
+      <c r="B19" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4113,11 +3862,11 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="83" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>49</v>
+      <c r="A20" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C20">
         <v>1.004110395096911</v>
@@ -4133,9 +3882,9 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="83"/>
-      <c r="B21" s="24" t="s">
-        <v>50</v>
+      <c r="A21" s="77"/>
+      <c r="B21" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4169,9 +3918,9 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="83"/>
-      <c r="B22" s="24" t="s">
-        <v>51</v>
+      <c r="A22" s="77"/>
+      <c r="B22" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -4205,11 +3954,11 @@
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>49</v>
+      <c r="A23" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C23">
         <v>1.013993382565658</v>
@@ -4225,9 +3974,9 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="83"/>
-      <c r="B24" s="24" t="s">
-        <v>50</v>
+      <c r="A24" s="77"/>
+      <c r="B24" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -4242,84 +3991,102 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <v>0.89356372527232952</v>
+        <v>0.87339073337913475</v>
       </c>
       <c r="H24">
-        <v>0.94572412477475598</v>
+        <v>0.92074759596716416</v>
       </c>
       <c r="I24">
-        <v>0.96700588431045986</v>
+        <v>0.95058492075138856</v>
       </c>
       <c r="J24">
-        <v>0.95620143147246406</v>
+        <v>0.95791588696615193</v>
       </c>
       <c r="K24">
-        <v>0.94117637444183477</v>
+        <v>0.95501099482379692</v>
       </c>
       <c r="L24">
-        <v>1.004745470365263</v>
+        <v>1.0074311136596641</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="83"/>
-      <c r="B25" s="24" t="s">
-        <v>51</v>
+      <c r="A25" s="77"/>
+      <c r="B25" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C25">
-        <v>1.094033662264088</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.97947807743700044</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.97401476390684771</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>0.97345171255326479</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0.84493275045896465</v>
+        <v>0.86910210149954803</v>
       </c>
       <c r="H25">
-        <v>0.89923971011504922</v>
+        <v>0.91197560070142802</v>
       </c>
       <c r="I25">
-        <v>0.91238917500026184</v>
+        <v>0.93739798411844588</v>
       </c>
       <c r="J25">
-        <v>0.91549146302094686</v>
+        <v>0.9395616359029878</v>
       </c>
       <c r="K25">
-        <v>0.90476275832553921</v>
+        <v>0.93353918965308891</v>
       </c>
       <c r="L25">
-        <v>0.95524557678015487</v>
+        <v>0.98065537933534308</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>49</v>
+      <c r="A26" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>57</v>
       </c>
       <c r="C26">
         <v>0.9901150705631423</v>
       </c>
       <c r="D26">
-        <v>0.86424547635730642</v>
+        <v>0.8642454763573062</v>
       </c>
       <c r="E26">
-        <v>0.93931372717126993</v>
+        <v>0.93931372717126982</v>
       </c>
       <c r="F26">
         <v>0.89538487727018501</v>
       </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="83"/>
-      <c r="B27" s="24" t="s">
-        <v>50</v>
+      <c r="A27" s="77"/>
+      <c r="B27" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -4334,58 +4101,58 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>0.87215669335447066</v>
+        <v>0.85903936299714301</v>
       </c>
       <c r="H27">
-        <v>0.90613687436761492</v>
+        <v>0.89485678551708547</v>
       </c>
       <c r="I27">
-        <v>0.95735635458034407</v>
+        <v>0.94662610516975831</v>
       </c>
       <c r="J27">
-        <v>0.95045833770876909</v>
+        <v>0.95157129206988267</v>
       </c>
       <c r="K27">
-        <v>0.95447768841398661</v>
+        <v>0.96348256887667472</v>
       </c>
       <c r="L27">
-        <v>1.013103464315301</v>
+        <v>1.0143159164944151</v>
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="83"/>
-      <c r="B28" s="24" t="s">
-        <v>51</v>
+      <c r="A28" s="77"/>
+      <c r="B28" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="C28">
-        <v>1.0612060081721459</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0.99073523658819929</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0.9830448659775618</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>0.98279129183062408</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0.817604109991656</v>
+        <v>0.83332004165911022</v>
       </c>
       <c r="H28">
-        <v>0.83621131789626324</v>
+        <v>0.84196319713103152</v>
       </c>
       <c r="I28">
-        <v>0.8959308898051539</v>
+        <v>0.91227285161114025</v>
       </c>
       <c r="J28">
-        <v>0.89935761689068849</v>
+        <v>0.91498298831646119</v>
       </c>
       <c r="K28">
-        <v>0.90409275487043739</v>
+        <v>0.92282318021591314</v>
       </c>
       <c r="L28">
-        <v>0.95579981083366627</v>
+        <v>0.96727124136322284</v>
       </c>
     </row>
   </sheetData>
@@ -4402,4 +4169,310 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="60">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="60">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="60">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>19922.471000000001</v>
+      </c>
+      <c r="C2">
+        <v>3073.877410478342</v>
+      </c>
+      <c r="D2">
+        <v>19816.433954755132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>526058.97600000002</v>
+      </c>
+      <c r="C3">
+        <v>513128.15045075922</v>
+      </c>
+      <c r="D3">
+        <v>539850.19252898183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>47354.067999999999</v>
+      </c>
+      <c r="C4">
+        <v>63119.264660570007</v>
+      </c>
+      <c r="D4">
+        <v>69747.17724995059</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>81377.207999999999</v>
+      </c>
+      <c r="C5">
+        <v>52058.778690093699</v>
+      </c>
+      <c r="D5">
+        <v>83160.913900785905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>311336.77399999998</v>
+      </c>
+      <c r="C6">
+        <v>332277.71716741187</v>
+      </c>
+      <c r="D6">
+        <v>358563.77458584151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>329466.32699999999</v>
+      </c>
+      <c r="C7">
+        <v>321864.84933468088</v>
+      </c>
+      <c r="D7">
+        <v>339683.71317785408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>71176.005999999994</v>
+      </c>
+      <c r="C8">
+        <v>67932.599728931222</v>
+      </c>
+      <c r="D8">
+        <v>74103.478048825011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>2132447.2349999999</v>
+      </c>
+      <c r="C9">
+        <v>1962993.1692271589</v>
+      </c>
+      <c r="D9">
+        <v>2094345.8161026461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>3519139.0649999999</v>
+      </c>
+      <c r="C10">
+        <v>3316448.4066700842</v>
+      </c>
+      <c r="D10">
+        <v>3579271.4995496399</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="60">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="60">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="60">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>19922.471000000001</v>
+      </c>
+      <c r="C2">
+        <v>2372.2827102244878</v>
+      </c>
+      <c r="D2">
+        <v>15258.296771098911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>526058.97600000002</v>
+      </c>
+      <c r="C3">
+        <v>478518.61148725299</v>
+      </c>
+      <c r="D3">
+        <v>514143.04050379217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>47354.067999999999</v>
+      </c>
+      <c r="C4">
+        <v>52771.23810704668</v>
+      </c>
+      <c r="D4">
+        <v>65543.827594732618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>81377.207999999999</v>
+      </c>
+      <c r="C5">
+        <v>49121.780516297891</v>
+      </c>
+      <c r="D5">
+        <v>70653.884547747002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>311336.77399999998</v>
+      </c>
+      <c r="C6">
+        <v>309309.16141848691</v>
+      </c>
+      <c r="D6">
+        <v>313694.55911220011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>329466.32699999999</v>
+      </c>
+      <c r="C7">
+        <v>317542.43237850227</v>
+      </c>
+      <c r="D7">
+        <v>328491.53624475643</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>71176.005999999994</v>
+      </c>
+      <c r="C8">
+        <v>66080.899188435054</v>
+      </c>
+      <c r="D8">
+        <v>71863.599382376968</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>2132447.2349999999</v>
+      </c>
+      <c r="C9">
+        <v>1955840.2836242591</v>
+      </c>
+      <c r="D9">
+        <v>2051070.841844277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>3519139.0649999999</v>
+      </c>
+      <c r="C10">
+        <v>3231556.689430506</v>
+      </c>
+      <c r="D10">
+        <v>3430719.5860009808</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>